<commit_message>
Water model update and general updates
</commit_message>
<xml_diff>
--- a/Data/The Three Scenarios.xlsx
+++ b/Data/The Three Scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvjos\Desktop\System\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DORHEN\Desktop\Research-Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C1FB77-35B1-4FAD-A8EC-8F0214CA9C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B9E8B8-4C43-4918-A163-9C547DE7A5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="4410" windowWidth="27705" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -47,6 +47,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>talcordo@post.bgu.ac.il:</t>
         </r>
@@ -55,6 +56,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 ההערכה היא ש-33% מהמזון נזרק.
@@ -70,6 +72,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>talcordo@post.bgu.ac.il:</t>
         </r>
@@ -78,6 +81,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 יש נתונים לגבי הפליטות של רכבים עם שיפורי פליטות</t>
@@ -453,16 +457,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -471,7 +475,7 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -479,21 +483,21 @@
       <b/>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -502,18 +506,20 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -521,14 +527,14 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -536,7 +542,7 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -830,9 +836,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -889,7 +895,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -904,11 +909,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="7" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="7" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -923,7 +928,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="14" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="14" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -958,9 +963,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -998,9 +1003,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1033,26 +1038,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1085,26 +1073,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1280,19 +1251,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1322,7 +1293,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1354,7 +1325,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1386,7 +1357,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1418,7 +1389,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
@@ -1434,23 +1405,23 @@
       <c r="E5" s="16">
         <v>0</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="19">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="19">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="19">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="19">
         <v>0.28000000000000003</v>
       </c>
       <c r="J5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
@@ -1466,23 +1437,23 @@
       <c r="E6" s="16">
         <v>0.33</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="19">
         <v>0.16</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="19">
         <v>0.16</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="19">
         <v>0.16</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="19">
         <v>0.08</v>
       </c>
       <c r="J6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
@@ -1495,7 +1466,7 @@
       <c r="D7" s="5">
         <v>0.32</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="21">
         <v>0.06</v>
       </c>
       <c r="F7" s="19">
@@ -1514,7 +1485,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
@@ -1546,7 +1517,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
@@ -1562,23 +1533,23 @@
       <c r="E9" s="16">
         <v>0</v>
       </c>
-      <c r="F9" s="20">
-        <v>0</v>
-      </c>
-      <c r="G9" s="20">
-        <v>0</v>
-      </c>
-      <c r="H9" s="20">
+      <c r="F9" s="19">
+        <v>0</v>
+      </c>
+      <c r="G9" s="19">
+        <v>0</v>
+      </c>
+      <c r="H9" s="19">
         <v>0.05</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="19">
         <v>0.16</v>
       </c>
       <c r="J9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
@@ -1594,24 +1565,24 @@
       <c r="E10" s="16">
         <v>0</v>
       </c>
-      <c r="F10" s="20">
-        <v>0</v>
-      </c>
-      <c r="G10" s="20">
-        <v>0</v>
-      </c>
-      <c r="H10" s="20">
-        <v>0</v>
-      </c>
-      <c r="I10" s="20">
+      <c r="F10" s="19">
+        <v>0</v>
+      </c>
+      <c r="G10" s="19">
+        <v>0</v>
+      </c>
+      <c r="H10" s="19">
+        <v>0</v>
+      </c>
+      <c r="I10" s="19">
         <v>0</v>
       </c>
       <c r="J10" t="s">
         <v>113</v>
       </c>
-      <c r="K10" s="27"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="26"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>111</v>
       </c>
@@ -1627,23 +1598,23 @@
       <c r="E11" s="16">
         <v>0</v>
       </c>
-      <c r="F11" s="20">
-        <v>0</v>
-      </c>
-      <c r="G11" s="20">
-        <v>0</v>
-      </c>
-      <c r="H11" s="20">
-        <v>0</v>
-      </c>
-      <c r="I11" s="20">
+      <c r="F11" s="19">
+        <v>0</v>
+      </c>
+      <c r="G11" s="19">
+        <v>0</v>
+      </c>
+      <c r="H11" s="19">
+        <v>0</v>
+      </c>
+      <c r="I11" s="19">
         <v>0</v>
       </c>
       <c r="J11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>11</v>
       </c>
@@ -1659,23 +1630,23 @@
       <c r="E12" s="16">
         <v>0</v>
       </c>
-      <c r="F12" s="20">
-        <v>0</v>
-      </c>
-      <c r="G12" s="20">
-        <v>0</v>
-      </c>
-      <c r="H12" s="20">
-        <v>0</v>
-      </c>
-      <c r="I12" s="20">
+      <c r="F12" s="19">
+        <v>0</v>
+      </c>
+      <c r="G12" s="19">
+        <v>0</v>
+      </c>
+      <c r="H12" s="19">
+        <v>0</v>
+      </c>
+      <c r="I12" s="19">
         <v>0</v>
       </c>
       <c r="J12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>12</v>
       </c>
@@ -1691,23 +1662,23 @@
       <c r="E13" s="16">
         <v>0</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="19">
         <v>0.2</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G13" s="19">
         <v>0.2</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="19">
         <v>0.2</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="19">
         <v>0.3</v>
       </c>
       <c r="J13" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>13</v>
       </c>
@@ -1723,23 +1694,23 @@
       <c r="E14" s="16">
         <v>0</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="19">
         <v>0.25</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="19">
         <v>0.25</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="19">
         <v>0.25</v>
       </c>
-      <c r="I14" s="20">
+      <c r="I14" s="19">
         <v>0.5</v>
       </c>
       <c r="J14" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>14</v>
       </c>
@@ -1755,23 +1726,23 @@
       <c r="E15" s="16">
         <v>0</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="19">
         <v>1</v>
       </c>
-      <c r="G15" s="20">
+      <c r="G15" s="19">
         <v>1</v>
       </c>
-      <c r="H15" s="20">
+      <c r="H15" s="19">
         <v>1</v>
       </c>
-      <c r="I15" s="20">
+      <c r="I15" s="19">
         <v>1</v>
       </c>
       <c r="J15" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>15</v>
       </c>
@@ -1787,23 +1758,23 @@
       <c r="E16" s="16">
         <v>0</v>
       </c>
-      <c r="F16" s="20">
-        <v>0</v>
-      </c>
-      <c r="G16" s="20">
-        <v>0</v>
-      </c>
-      <c r="H16" s="20">
+      <c r="F16" s="19">
+        <v>0</v>
+      </c>
+      <c r="G16" s="19">
+        <v>0</v>
+      </c>
+      <c r="H16" s="19">
         <v>0.1</v>
       </c>
-      <c r="I16" s="20">
+      <c r="I16" s="19">
         <v>0.3</v>
       </c>
       <c r="J16" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>26</v>
       </c>
@@ -1819,23 +1790,23 @@
       <c r="E17" s="16">
         <v>0</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="19">
         <v>0.25</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="19">
         <v>0.25</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H17" s="19">
         <v>0.1</v>
       </c>
-      <c r="I17" s="20">
+      <c r="I17" s="19">
         <v>0.25</v>
       </c>
       <c r="J17" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>16</v>
       </c>
@@ -1851,23 +1822,23 @@
       <c r="E18" s="16">
         <v>0</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="19">
         <v>1</v>
       </c>
-      <c r="G18" s="20">
+      <c r="G18" s="19">
         <v>1</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H18" s="19">
         <v>1</v>
       </c>
-      <c r="I18" s="20">
+      <c r="I18" s="19">
         <v>1</v>
       </c>
       <c r="J18" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
         <v>25</v>
       </c>
@@ -1883,23 +1854,23 @@
       <c r="E19" s="16">
         <v>0</v>
       </c>
-      <c r="F19" s="20">
-        <v>0</v>
-      </c>
-      <c r="G19" s="20">
-        <v>0</v>
-      </c>
-      <c r="H19" s="20">
-        <v>0</v>
-      </c>
-      <c r="I19" s="20">
+      <c r="F19" s="19">
+        <v>0</v>
+      </c>
+      <c r="G19" s="19">
+        <v>0</v>
+      </c>
+      <c r="H19" s="19">
+        <v>0</v>
+      </c>
+      <c r="I19" s="19">
         <v>0</v>
       </c>
       <c r="J19" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>17</v>
       </c>
@@ -1915,16 +1886,16 @@
       <c r="E20" s="16">
         <v>0</v>
       </c>
-      <c r="F20" s="20">
-        <v>0</v>
-      </c>
-      <c r="G20" s="20">
-        <v>0</v>
-      </c>
-      <c r="H20" s="20">
-        <v>0</v>
-      </c>
-      <c r="I20" s="20">
+      <c r="F20" s="19">
+        <v>0</v>
+      </c>
+      <c r="G20" s="19">
+        <v>0</v>
+      </c>
+      <c r="H20" s="19">
+        <v>0</v>
+      </c>
+      <c r="I20" s="19">
         <v>0.1</v>
       </c>
       <c r="J20" t="s">
@@ -1945,47 +1916,47 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27" style="21" customWidth="1"/>
+    <col min="2" max="2" width="27" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="37"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="B1" s="36"/>
+    </row>
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="B2" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="B3" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="23">
         <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="25">
         <v>0</v>
       </c>
     </row>
@@ -2006,396 +1977,396 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.375" customWidth="1"/>
+    <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="D1" s="38" t="s">
+      <c r="B1" s="37"/>
+      <c r="D1" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="38"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="E1" s="37"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="31" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="31" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D6" s="32" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6" s="31" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="D7" s="33" t="s">
+      <c r="B7" s="37"/>
+      <c r="D7" s="32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="31" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="31" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="34" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="35" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D13" s="34" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="D14" s="35" t="s">
+      <c r="B14" s="37"/>
+      <c r="D14" s="34" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="34" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="31" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="31" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="33" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="31" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="31" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D22" s="34" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D22" s="33" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="34" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="33" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="34" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="33" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D25" s="34" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D25" s="33" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D26" s="34" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="33" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D27" s="34" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D27" s="33" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D28" s="34" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D28" s="33" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D29" s="34" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D29" s="33" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D30" s="34" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D30" s="33" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D31" s="34" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D31" s="33" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D32" s="34" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D32" s="33" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="34" t="s">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="33" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34" s="34" t="s">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D34" s="33" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D35" s="34" t="s">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D35" s="33" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="34" t="s">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D36" s="33" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="34" t="s">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D37" s="33" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="34" t="s">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D38" s="33" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D39" s="34" t="s">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D39" s="33" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D40" s="34" t="s">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D40" s="33" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D41" s="34" t="s">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D41" s="33" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D42" s="34" t="s">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D42" s="33" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D43" s="34" t="s">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D43" s="33" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D44" s="34" t="s">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D44" s="33" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D45" s="34" t="s">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D45" s="33" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D46" s="34" t="s">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D46" s="33" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D47" s="34" t="s">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D47" s="33" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D48" s="34" t="s">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D48" s="33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="34" t="s">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D49" s="33" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D50" s="34" t="s">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D50" s="33" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D51" s="34" t="s">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D51" s="33" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="34" t="s">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D52" s="33" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53" s="34" t="s">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D53" s="33" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D54" s="34" t="s">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D54" s="33" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D55" s="34" t="s">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D55" s="33" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="34" t="s">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D56" s="33" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="34" t="s">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D57" s="33" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="34" t="s">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D58" s="33" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D59" s="34" t="s">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D59" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D60" s="34" t="s">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D60" s="33" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D61" s="34" t="s">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D61" s="33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D62" s="34" t="s">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D62" s="33" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D63" s="34" t="s">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D63" s="33" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D64" s="34" t="s">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D64" s="33" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="34" t="s">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D65" s="33" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing electricity form vehicles
</commit_message>
<xml_diff>
--- a/Data/The Three Scenarios.xlsx
+++ b/Data/The Three Scenarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DORHEN\Desktop\Research-Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B9E8B8-4C43-4918-A163-9C547DE7A5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72164AA2-54E1-470F-A050-FA026BD9A25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,12 +104,6 @@
     <t>s3</t>
   </si>
   <si>
-    <t>change in electricity consumption per capita in 2030</t>
-  </si>
-  <si>
-    <t>Change in desalinated water in 2030</t>
-  </si>
-  <si>
     <t>reducing beef consumption</t>
   </si>
   <si>
@@ -176,9 +170,6 @@
     <t xml:space="preserve"> electric truck vehicle</t>
   </si>
   <si>
-    <t xml:space="preserve">population growth by 2030 </t>
-  </si>
-  <si>
     <t>Electricity</t>
   </si>
   <si>
@@ -450,6 +441,15 @@
   </si>
   <si>
     <t>Advanced</t>
+  </si>
+  <si>
+    <t>population growth</t>
+  </si>
+  <si>
+    <t>change in electricity consumption per capita</t>
+  </si>
+  <si>
+    <t>Change in desalinated water</t>
   </si>
 </sst>
 </file>
@@ -1251,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1275,27 +1275,27 @@
         <v>2</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F1" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>118</v>
-      </c>
       <c r="J1" s="15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>116</v>
       </c>
       <c r="B2" s="4">
         <v>0</v>
@@ -1322,12 +1322,12 @@
         <v>0.9</v>
       </c>
       <c r="J2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>3</v>
+        <v>117</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -1354,12 +1354,12 @@
         <v>0.41</v>
       </c>
       <c r="J3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>4</v>
+        <v>118</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -1386,12 +1386,12 @@
         <v>2.64</v>
       </c>
       <c r="J4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
@@ -1418,12 +1418,12 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="J5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="17">
         <v>0</v>
@@ -1450,12 +1450,12 @@
         <v>0.08</v>
       </c>
       <c r="J6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4">
         <v>0.1</v>
@@ -1482,12 +1482,12 @@
         <v>0.8</v>
       </c>
       <c r="J7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="9">
         <v>0.63100000000000001</v>
@@ -1514,12 +1514,12 @@
         <v>0.2</v>
       </c>
       <c r="J8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4">
         <v>0.2</v>
@@ -1546,12 +1546,12 @@
         <v>0.16</v>
       </c>
       <c r="J9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4">
         <v>0</v>
@@ -1578,13 +1578,13 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B11" s="4">
         <v>0.51</v>
@@ -1611,12 +1611,12 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4">
         <v>0.26</v>
@@ -1643,12 +1643,12 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="4">
         <v>0</v>
@@ -1675,12 +1675,12 @@
         <v>0.3</v>
       </c>
       <c r="J13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="4">
         <v>0.04</v>
@@ -1707,12 +1707,12 @@
         <v>0.5</v>
       </c>
       <c r="J14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4">
         <v>0</v>
@@ -1739,12 +1739,12 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="4">
         <v>0</v>
@@ -1771,12 +1771,12 @@
         <v>0.3</v>
       </c>
       <c r="J16" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B17" s="4">
         <v>0</v>
@@ -1803,12 +1803,12 @@
         <v>0.25</v>
       </c>
       <c r="J17" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="4">
         <v>0</v>
@@ -1835,12 +1835,12 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" s="4">
         <v>0.75</v>
@@ -1867,12 +1867,12 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="4">
         <v>0.05</v>
@@ -1899,7 +1899,7 @@
         <v>0.1</v>
       </c>
       <c r="J20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1924,13 +1924,13 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="36"/>
     </row>
     <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="23">
         <v>0</v>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="23">
         <v>0</v>
@@ -1946,7 +1946,7 @@
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="23">
         <v>0.5</v>
@@ -1954,7 +1954,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" s="25">
         <v>0</v>
@@ -1986,388 +1986,388 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="37" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B1" s="37"/>
       <c r="D1" s="37" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D6" s="31" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" s="37"/>
       <c r="D7" s="32" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D13" s="34" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A14" s="37" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B14" s="37"/>
       <c r="D14" s="34" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="28" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="28" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D22" s="33" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D23" s="33" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D24" s="33" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D25" s="33" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D26" s="33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D27" s="33" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D28" s="33" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D29" s="33" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D30" s="33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D31" s="33" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D32" s="33" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D33" s="33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D34" s="33" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D35" s="33" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D36" s="33" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D37" s="33" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D38" s="33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D39" s="33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D40" s="33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D41" s="33" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D42" s="33" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D43" s="33" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D44" s="33" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D45" s="33" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D46" s="33" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D47" s="33" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D48" s="33" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D49" s="33" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D50" s="33" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D51" s="33" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D52" s="33" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D53" s="33" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D54" s="33" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D55" s="33" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D56" s="33" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D57" s="33" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D58" s="33" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D59" s="33" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D60" s="33" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D61" s="33" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D62" s="33" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D63" s="33" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D64" s="33" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D65" s="33" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding industrial fuels to the model
</commit_message>
<xml_diff>
--- a/Data/The Three Scenarios.xlsx
+++ b/Data/The Three Scenarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DORHEN\Desktop\Research-Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72164AA2-54E1-470F-A050-FA026BD9A25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948945F9-0893-4D7A-ADDB-B3D2E0FD62A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,9 +119,6 @@
     <t>electricity saving</t>
   </si>
   <si>
-    <t>waste minimization</t>
-  </si>
-  <si>
     <t>burning waste</t>
   </si>
   <si>
@@ -450,6 +447,9 @@
   </si>
   <si>
     <t>Change in desalinated water</t>
+  </si>
+  <si>
+    <t>fuel for energy</t>
   </si>
 </sst>
 </file>
@@ -1251,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1275,27 +1275,27 @@
         <v>2</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="15" t="s">
-        <v>115</v>
-      </c>
       <c r="J1" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="4">
         <v>0</v>
@@ -1322,12 +1322,12 @@
         <v>0.9</v>
       </c>
       <c r="J2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -1354,12 +1354,12 @@
         <v>0.41</v>
       </c>
       <c r="J3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -1386,7 +1386,7 @@
         <v>2.64</v>
       </c>
       <c r="J4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1418,7 +1418,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="J5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1450,7 +1450,7 @@
         <v>0.08</v>
       </c>
       <c r="J6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1482,7 +1482,7 @@
         <v>0.8</v>
       </c>
       <c r="J7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1514,7 +1514,7 @@
         <v>0.2</v>
       </c>
       <c r="J8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1546,12 +1546,12 @@
         <v>0.16</v>
       </c>
       <c r="J9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>8</v>
+        <v>118</v>
       </c>
       <c r="B10" s="4">
         <v>0</v>
@@ -1560,7 +1560,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="5">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="E10" s="16">
         <v>0</v>
@@ -1572,19 +1572,19 @@
         <v>0</v>
       </c>
       <c r="H10" s="19">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I10" s="19">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="J10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B11" s="4">
         <v>0.51</v>
@@ -1611,12 +1611,12 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="4">
         <v>0.26</v>
@@ -1643,12 +1643,12 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="4">
         <v>0</v>
@@ -1675,12 +1675,12 @@
         <v>0.3</v>
       </c>
       <c r="J13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="4">
         <v>0.04</v>
@@ -1707,12 +1707,12 @@
         <v>0.5</v>
       </c>
       <c r="J14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="4">
         <v>0</v>
@@ -1739,12 +1739,12 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="4">
         <v>0</v>
@@ -1771,12 +1771,12 @@
         <v>0.3</v>
       </c>
       <c r="J16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="4">
         <v>0</v>
@@ -1803,12 +1803,12 @@
         <v>0.25</v>
       </c>
       <c r="J17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="4">
         <v>0</v>
@@ -1835,12 +1835,12 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="4">
         <v>0.75</v>
@@ -1867,12 +1867,12 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="4">
         <v>0.05</v>
@@ -1899,7 +1899,7 @@
         <v>0.1</v>
       </c>
       <c r="J20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1924,13 +1924,13 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="36"/>
     </row>
     <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="23">
         <v>0</v>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="23">
         <v>0</v>
@@ -1946,7 +1946,7 @@
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="23">
         <v>0.5</v>
@@ -1954,7 +1954,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="25">
         <v>0</v>
@@ -1986,388 +1986,388 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="37"/>
       <c r="D1" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D6" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="37"/>
       <c r="D7" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D13" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A14" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="37"/>
       <c r="D14" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D22" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D23" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D24" s="33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D25" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D26" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D27" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D28" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D29" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D30" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D31" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D32" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D33" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D34" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D35" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D36" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D37" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D38" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D39" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D40" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D41" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D42" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D43" s="33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D44" s="33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D45" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D46" s="33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D47" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D48" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D49" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D50" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D51" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D52" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D53" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D54" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D55" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D56" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D57" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D58" s="33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D59" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D60" s="33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D61" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D62" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D63" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D64" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D65" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
preperations for 2035 scenarios
</commit_message>
<xml_diff>
--- a/Data/The Three Scenarios.xlsx
+++ b/Data/The Three Scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DORHEN\Desktop\Shared-Project\NewVersion\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LAB\April 2024 Version\Research-Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CAA40C-90EF-4A2A-863D-C102D59A3048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51799D45-4178-4587-B418-448980D3DBFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="120">
   <si>
     <t>s1</t>
   </si>
@@ -450,6 +450,9 @@
   </si>
   <si>
     <t>fuel for energy</t>
+  </si>
+  <si>
+    <t>New</t>
   </si>
 </sst>
 </file>
@@ -466,7 +469,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -475,7 +478,7 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -483,21 +486,21 @@
       <b/>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -519,7 +522,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -527,14 +530,14 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -542,12 +545,12 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -632,6 +635,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -838,7 +847,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -904,7 +913,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -933,6 +941,10 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1249,21 +1261,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="22.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1274,7 +1286,7 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="35" t="s">
         <v>15</v>
       </c>
       <c r="F1" s="15" t="s">
@@ -1283,17 +1295,20 @@
       <c r="G1" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="35" t="s">
         <v>114</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="K1" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>115</v>
       </c>
@@ -1324,8 +1339,12 @@
       <c r="J2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K2" s="19">
+        <v>0.41</v>
+      </c>
+      <c r="L2" s="19"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>116</v>
       </c>
@@ -1356,8 +1375,12 @@
       <c r="J3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K3" s="19">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="L3" s="19"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>117</v>
       </c>
@@ -1388,8 +1411,12 @@
       <c r="J4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K4" s="19">
+        <v>2.64</v>
+      </c>
+      <c r="L4" s="19"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -1420,8 +1447,12 @@
       <c r="J5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K5" s="19">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L5" s="19"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -1452,8 +1483,12 @@
       <c r="J6" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="19"/>
+    </row>
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -1484,8 +1519,12 @@
       <c r="J7" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K7" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="L7" s="19"/>
+    </row>
+    <row r="8" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
@@ -1516,8 +1555,12 @@
       <c r="J8" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K8" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="L8" s="19"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -1548,8 +1591,12 @@
       <c r="J9" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K9" s="19">
+        <v>0.16</v>
+      </c>
+      <c r="L9" s="19"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>118</v>
       </c>
@@ -1580,9 +1627,12 @@
       <c r="J10" t="s">
         <v>109</v>
       </c>
-      <c r="K10" s="26"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K10" s="19">
+        <v>0.9</v>
+      </c>
+      <c r="L10" s="19"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>107</v>
       </c>
@@ -1613,8 +1663,12 @@
       <c r="J11" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K11" s="19">
+        <v>0</v>
+      </c>
+      <c r="L11" s="19"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
@@ -1645,8 +1699,12 @@
       <c r="J12" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K12" s="19">
+        <v>0</v>
+      </c>
+      <c r="L12" s="19"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>9</v>
       </c>
@@ -1677,8 +1735,12 @@
       <c r="J13" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K13" s="19">
+        <v>0.15</v>
+      </c>
+      <c r="L13" s="19"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>10</v>
       </c>
@@ -1709,8 +1771,12 @@
       <c r="J14" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K14" s="19">
+        <v>0.25</v>
+      </c>
+      <c r="L14" s="19"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>11</v>
       </c>
@@ -1741,8 +1807,12 @@
       <c r="J15" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K15" s="19">
+        <v>0.35</v>
+      </c>
+      <c r="L15" s="19"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>12</v>
       </c>
@@ -1773,8 +1843,12 @@
       <c r="J16" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="L16" s="19"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>23</v>
       </c>
@@ -1805,8 +1879,12 @@
       <c r="J17" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="L17" s="19"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>13</v>
       </c>
@@ -1837,8 +1915,12 @@
       <c r="J18" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="19">
+        <v>0.25</v>
+      </c>
+      <c r="L18" s="19"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>22</v>
       </c>
@@ -1869,8 +1951,12 @@
       <c r="J19" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="19">
+        <v>0</v>
+      </c>
+      <c r="L19" s="19"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>14</v>
       </c>
@@ -1901,6 +1987,10 @@
       <c r="J20" t="s">
         <v>109</v>
       </c>
+      <c r="K20" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="L20" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1912,23 +2002,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="36"/>
-    </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B1" s="37"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>18</v>
       </c>
@@ -1936,7 +2026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>19</v>
       </c>
@@ -1944,7 +2034,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>20</v>
       </c>
@@ -1952,7 +2042,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
         <v>21</v>
       </c>
@@ -1977,396 +2067,396 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.375" customWidth="1"/>
-    <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="D1" s="37" t="s">
+      <c r="B1" s="38"/>
+      <c r="D1" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="37"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="E1" s="38"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="30" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="30" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D6" s="31" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D6" s="30" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A7" s="37" t="s">
+    <row r="7" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="D7" s="32" t="s">
+      <c r="B7" s="38"/>
+      <c r="D7" s="31" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="32" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="30" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D13" s="34" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D13" s="33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A14" s="37" t="s">
+    <row r="14" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A14" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="D14" s="34" t="s">
+      <c r="B14" s="38"/>
+      <c r="D14" s="33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="28" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="30" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="28" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="30" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="28" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="28" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="30" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="29" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D22" s="33" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="32" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D23" s="33" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D23" s="32" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D24" s="33" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D24" s="32" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D25" s="33" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D25" s="32" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D26" s="33" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D26" s="32" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D27" s="33" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D27" s="32" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D28" s="33" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D28" s="32" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D29" s="33" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D29" s="32" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D30" s="33" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D30" s="32" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D31" s="33" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D31" s="32" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D32" s="33" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D32" s="32" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D33" s="33" t="s">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" s="32" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D34" s="33" t="s">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" s="32" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D35" s="33" t="s">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D35" s="32" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D36" s="33" t="s">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D36" s="32" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D37" s="33" t="s">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D37" s="32" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D38" s="33" t="s">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D38" s="32" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D39" s="33" t="s">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D39" s="32" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D40" s="33" t="s">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D40" s="32" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D41" s="33" t="s">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D41" s="32" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D42" s="33" t="s">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D42" s="32" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D43" s="33" t="s">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D43" s="32" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D44" s="33" t="s">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D44" s="32" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D45" s="33" t="s">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D45" s="32" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D46" s="33" t="s">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D46" s="32" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D47" s="33" t="s">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D47" s="32" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D48" s="33" t="s">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D48" s="32" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D49" s="33" t="s">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D49" s="32" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D50" s="33" t="s">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D50" s="32" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D51" s="33" t="s">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D51" s="32" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D52" s="33" t="s">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D52" s="32" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D53" s="33" t="s">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D53" s="32" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D54" s="33" t="s">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D54" s="32" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D55" s="33" t="s">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D55" s="32" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D56" s="33" t="s">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D56" s="32" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D57" s="33" t="s">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D57" s="32" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D58" s="33" t="s">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D58" s="32" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D59" s="33" t="s">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D59" s="32" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D60" s="33" t="s">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D60" s="32" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D61" s="33" t="s">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D61" s="32" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D62" s="33" t="s">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D62" s="32" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D63" s="33" t="s">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D63" s="32" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D64" s="33" t="s">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D64" s="32" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D65" s="33" t="s">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D65" s="32" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing 2035 calculations, sensitivity analysis
</commit_message>
<xml_diff>
--- a/Data/The Three Scenarios.xlsx
+++ b/Data/The Three Scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LAB\April 2024 Version\Research-Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51799D45-4178-4587-B418-448980D3DBFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BF01A9-E390-4FAA-B8C6-3A249D046858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="121">
   <si>
     <t>s1</t>
   </si>
@@ -453,6 +453,9 @@
   </si>
   <si>
     <t>New</t>
+  </si>
+  <si>
+    <t>reducing meat consumption</t>
   </si>
 </sst>
 </file>
@@ -847,7 +850,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -942,10 +945,15 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -955,6 +963,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 5" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1261,10 +1270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1272,10 +1281,9 @@
     <col min="1" max="1" width="47.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="22.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="22.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1286,7 +1294,7 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="34" t="s">
         <v>15</v>
       </c>
       <c r="F1" s="15" t="s">
@@ -1295,20 +1303,20 @@
       <c r="G1" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="34" t="s">
         <v>114</v>
       </c>
       <c r="J1" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="K1" s="15" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>115</v>
       </c>
@@ -1336,15 +1344,14 @@
       <c r="I2" s="19">
         <v>0.9</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="19">
+        <v>0.41</v>
+      </c>
+      <c r="K2" t="s">
         <v>109</v>
       </c>
-      <c r="K2" s="19">
-        <v>0.41</v>
-      </c>
-      <c r="L2" s="19"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>116</v>
       </c>
@@ -1372,15 +1379,14 @@
       <c r="I3" s="19">
         <v>0.41</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="19">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="K3" t="s">
         <v>109</v>
       </c>
-      <c r="K3" s="19">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="L3" s="19"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>117</v>
       </c>
@@ -1408,15 +1414,14 @@
       <c r="I4" s="19">
         <v>2.64</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="19">
+        <v>2.64</v>
+      </c>
+      <c r="K4" t="s">
         <v>109</v>
       </c>
-      <c r="K4" s="19">
-        <v>2.64</v>
-      </c>
-      <c r="L4" s="19"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -1444,15 +1449,14 @@
       <c r="I5" s="19">
         <v>0.28000000000000003</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="19">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K5" t="s">
         <v>110</v>
       </c>
-      <c r="K5" s="19">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="L5" s="19"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -1480,15 +1484,14 @@
       <c r="I6" s="19">
         <v>0.08</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="40">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="K6" t="s">
         <v>110</v>
       </c>
-      <c r="K6" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="L6" s="19"/>
-    </row>
-    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -1516,15 +1519,14 @@
       <c r="I7" s="19">
         <v>0.8</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="K7" t="s">
         <v>110</v>
       </c>
-      <c r="K7" s="19">
-        <v>0.4</v>
-      </c>
-      <c r="L7" s="19"/>
-    </row>
-    <row r="8" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
@@ -1552,15 +1554,14 @@
       <c r="I8" s="19">
         <v>0.2</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="K8" t="s">
         <v>110</v>
       </c>
-      <c r="K8" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="L8" s="19"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -1588,15 +1589,14 @@
       <c r="I9" s="19">
         <v>0.16</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="19">
+        <v>0.16</v>
+      </c>
+      <c r="K9" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="19">
-        <v>0.16</v>
-      </c>
-      <c r="L9" s="19"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>118</v>
       </c>
@@ -1624,15 +1624,14 @@
       <c r="I10" s="19">
         <v>0.9</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="19">
+        <v>0.9</v>
+      </c>
+      <c r="K10" t="s">
         <v>109</v>
       </c>
-      <c r="K10" s="19">
-        <v>0.9</v>
-      </c>
-      <c r="L10" s="19"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>107</v>
       </c>
@@ -1660,15 +1659,14 @@
       <c r="I11" s="19">
         <v>0</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="19">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
         <v>110</v>
       </c>
-      <c r="K11" s="19">
-        <v>0</v>
-      </c>
-      <c r="L11" s="19"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
@@ -1696,15 +1694,14 @@
       <c r="I12" s="19">
         <v>0</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="19">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
         <v>110</v>
       </c>
-      <c r="K12" s="19">
-        <v>0</v>
-      </c>
-      <c r="L12" s="19"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>9</v>
       </c>
@@ -1732,15 +1729,14 @@
       <c r="I13" s="19">
         <v>0.3</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="19">
+        <v>0.15</v>
+      </c>
+      <c r="K13" t="s">
         <v>109</v>
       </c>
-      <c r="K13" s="19">
-        <v>0.15</v>
-      </c>
-      <c r="L13" s="19"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>10</v>
       </c>
@@ -1768,15 +1764,14 @@
       <c r="I14" s="19">
         <v>0.5</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="19">
+        <v>0.25</v>
+      </c>
+      <c r="K14" t="s">
         <v>109</v>
       </c>
-      <c r="K14" s="19">
-        <v>0.25</v>
-      </c>
-      <c r="L14" s="19"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>11</v>
       </c>
@@ -1804,15 +1799,14 @@
       <c r="I15" s="19">
         <v>1</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="19">
+        <v>0.35</v>
+      </c>
+      <c r="K15" t="s">
         <v>110</v>
       </c>
-      <c r="K15" s="19">
-        <v>0.35</v>
-      </c>
-      <c r="L15" s="19"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>12</v>
       </c>
@@ -1840,15 +1834,14 @@
       <c r="I16" s="19">
         <v>0.3</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="K16" t="s">
         <v>110</v>
       </c>
-      <c r="K16" s="19">
-        <v>0.3</v>
-      </c>
-      <c r="L16" s="19"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>23</v>
       </c>
@@ -1876,15 +1869,14 @@
       <c r="I17" s="19">
         <v>0.25</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="K17" t="s">
         <v>110</v>
       </c>
-      <c r="K17" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="L17" s="19"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>13</v>
       </c>
@@ -1912,15 +1904,14 @@
       <c r="I18" s="19">
         <v>1</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="19">
+        <v>0.25</v>
+      </c>
+      <c r="K18" t="s">
         <v>110</v>
       </c>
-      <c r="K18" s="19">
-        <v>0.25</v>
-      </c>
-      <c r="L18" s="19"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>22</v>
       </c>
@@ -1948,15 +1939,14 @@
       <c r="I19" s="19">
         <v>0</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="19">
+        <v>0</v>
+      </c>
+      <c r="K19" t="s">
         <v>110</v>
       </c>
-      <c r="K19" s="19">
-        <v>0</v>
-      </c>
-      <c r="L19" s="19"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>14</v>
       </c>
@@ -1984,13 +1974,44 @@
       <c r="I20" s="19">
         <v>0.1</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="K20" t="s">
         <v>109</v>
       </c>
-      <c r="K20" s="19">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="35">
+        <v>0</v>
+      </c>
+      <c r="C21" s="36">
+        <v>0</v>
+      </c>
+      <c r="D21" s="36">
+        <v>0</v>
+      </c>
+      <c r="E21" s="16">
+        <v>0</v>
+      </c>
+      <c r="F21" s="19">
+        <v>0</v>
+      </c>
+      <c r="G21" s="19">
+        <v>0</v>
+      </c>
+      <c r="H21" s="19">
+        <v>0</v>
+      </c>
+      <c r="I21" s="19">
+        <v>0</v>
+      </c>
+      <c r="J21" s="19">
         <v>0.1</v>
       </c>
-      <c r="L20" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2013,10 +2034,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="38"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
@@ -2075,14 +2096,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="D1" s="38" t="s">
+      <c r="B1" s="39"/>
+      <c r="D1" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="38"/>
+      <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
@@ -2122,10 +2143,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="38"/>
+      <c r="B7" s="39"/>
       <c r="D7" s="31" t="s">
         <v>48</v>
       </c>
@@ -2176,10 +2197,10 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="38"/>
+      <c r="B14" s="39"/>
       <c r="D14" s="33" t="s">
         <v>55</v>
       </c>

</xml_diff>